<commit_message>
add time to shakeflask data, draft fermentation report
</commit_message>
<xml_diff>
--- a/protein_prod/data/class_shakeflask.xlsx
+++ b/protein_prod/data/class_shakeflask.xlsx
@@ -114,7 +114,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,12 +132,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -169,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -186,14 +180,11 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -222,7 +213,7 @@
       <totalsRowFormula>Sum</totalsRowFormula>
     </tableColumn>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showColumnStripes="0" showRowStripes="1" showLastColumn="0" showFirstColumn="0"/>
+  <tableStyleInfo name="TableStyleLight1" showColumnStripes="0" showRowStripes="1" showLastColumn="0" showFirstColumn="0"/>
 </table>
 </file>
 
@@ -520,12 +511,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="29.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="10.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="29.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="10.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -1048,7 +1039,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
@@ -1061,8 +1052,8 @@
       <c r="D27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="1" t="s">
@@ -1184,7 +1175,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="1" t="s">
         <v>25</v>
       </c>
@@ -1197,8 +1188,8 @@
       <c r="D34" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="1" t="s">
@@ -1333,8 +1324,8 @@
       <c r="D41" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>